<commit_message>
Cluster records list down completed
</commit_message>
<xml_diff>
--- a/test-output/e6dataTestOutput.xlsx
+++ b/test-output/e6dataTestOutput.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="83">
   <si>
     <t>Menu List</t>
   </si>
@@ -75,12 +75,205 @@
   </si>
   <si>
     <t>Cluster</t>
+  </si>
+  <si>
+    <t>hive1</t>
+  </si>
+  <si>
+    <t>Ak-1</t>
+  </si>
+  <si>
+    <t>single-catalog</t>
+  </si>
+  <si>
+    <t>united</t>
+  </si>
+  <si>
+    <t>refreshcheck</t>
+  </si>
+  <si>
+    <t>rcg</t>
+  </si>
+  <si>
+    <t>catalog</t>
+  </si>
+  <si>
+    <t>metabase</t>
+  </si>
+  <si>
+    <t>rcg-unity</t>
+  </si>
+  <si>
+    <t>testhv</t>
+  </si>
+  <si>
+    <t>glue-22nd</t>
+  </si>
+  <si>
+    <t>glust</t>
+  </si>
+  <si>
+    <t>glue-21st</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>fresh-1</t>
+  </si>
+  <si>
+    <t>calatog</t>
+  </si>
+  <si>
+    <t>cata-auto</t>
+  </si>
+  <si>
+    <t>bi-test</t>
+  </si>
+  <si>
+    <t>naresh</t>
+  </si>
+  <si>
+    <t>bee</t>
+  </si>
+  <si>
+    <t>kpglue</t>
+  </si>
+  <si>
+    <t>newtest</t>
+  </si>
+  <si>
+    <t>partially</t>
+  </si>
+  <si>
+    <t>glueall</t>
+  </si>
+  <si>
+    <t>glu</t>
+  </si>
+  <si>
+    <t>chargebeetest</t>
+  </si>
+  <si>
+    <t>prodtetst2</t>
+  </si>
+  <si>
+    <t>producttest</t>
+  </si>
+  <si>
+    <t>srigluetest</t>
+  </si>
+  <si>
+    <t>jyoti@e6x.io</t>
+  </si>
+  <si>
+    <t>akash@e6x.io</t>
+  </si>
+  <si>
+    <t>govindaraju@e6x.io</t>
+  </si>
+  <si>
+    <t>kumar@e6x.io</t>
+  </si>
+  <si>
+    <t>rajath@e6x.io</t>
+  </si>
+  <si>
+    <t>garvit@e6x.io</t>
+  </si>
+  <si>
+    <t>shubham.kumar@e6x.io</t>
+  </si>
+  <si>
+    <t>dasari.laxminaresh@e6x.io</t>
+  </si>
+  <si>
+    <t>vishal@e6x.io</t>
+  </si>
+  <si>
+    <t>karan@e6x.io</t>
+  </si>
+  <si>
+    <t>srinath@e6x.io</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>feb-27th</t>
+  </si>
+  <si>
+    <t>highqps</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>testt</t>
+  </si>
+  <si>
+    <t>feb-24th</t>
+  </si>
+  <si>
+    <t>feb-7th</t>
+  </si>
+  <si>
+    <t>pov</t>
+  </si>
+  <si>
+    <t>task@e6x.io</t>
+  </si>
+  <si>
+    <t>shubham@e6x.io</t>
+  </si>
+  <si>
+    <t>Suspended</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>plt-infra</t>
+  </si>
+  <si>
+    <t>Query editor</t>
+  </si>
+  <si>
+    <t>Notebook</t>
+  </si>
+  <si>
+    <t>Catalogs</t>
+  </si>
+  <si>
+    <t>Clusters</t>
+  </si>
+  <si>
+    <t>Query history</t>
+  </si>
+  <si>
+    <t>Connectivity</t>
+  </si>
+  <si>
+    <t>Endpoints</t>
+  </si>
+  <si>
+    <t>IP sets</t>
+  </si>
+  <si>
+    <t>Workspaces</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -435,18 +628,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="20.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -457,7 +700,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -465,10 +708,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.0"/>
+    <col min="2" max="2" customWidth="true" width="24.5703125"/>
+    <col min="3" max="3" customWidth="true" width="19.42578125"/>
+    <col min="4" max="4" customWidth="true" width="22.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -483,6 +726,328 @@
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -492,7 +1057,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
@@ -500,10 +1065,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.0"/>
+    <col min="2" max="2" customWidth="true" width="24.5703125"/>
+    <col min="3" max="3" customWidth="true" width="19.42578125"/>
+    <col min="4" max="4" customWidth="true" width="22.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -518,6 +1083,119 @@
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -535,9 +1213,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.42578125"/>
+    <col min="2" max="2" customWidth="true" width="28.0"/>
+    <col min="3" max="3" customWidth="true" width="30.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -552,13 +1230,13 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed the Assignment and enabled to parallel
</commit_message>
<xml_diff>
--- a/test-output/e6dataTestOutput.xlsx
+++ b/test-output/e6dataTestOutput.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="83">
   <si>
     <t>Menu List</t>
   </si>
@@ -75,12 +75,205 @@
   </si>
   <si>
     <t>test (Glue)</t>
+  </si>
+  <si>
+    <t>hive1</t>
+  </si>
+  <si>
+    <t>Ak-1</t>
+  </si>
+  <si>
+    <t>single-catalog</t>
+  </si>
+  <si>
+    <t>united</t>
+  </si>
+  <si>
+    <t>refreshcheck</t>
+  </si>
+  <si>
+    <t>rcg</t>
+  </si>
+  <si>
+    <t>catalog</t>
+  </si>
+  <si>
+    <t>metabase</t>
+  </si>
+  <si>
+    <t>rcg-unity</t>
+  </si>
+  <si>
+    <t>testhv</t>
+  </si>
+  <si>
+    <t>glue-22nd</t>
+  </si>
+  <si>
+    <t>glust</t>
+  </si>
+  <si>
+    <t>glue-21st</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>fresh-1</t>
+  </si>
+  <si>
+    <t>calatog</t>
+  </si>
+  <si>
+    <t>cata-auto</t>
+  </si>
+  <si>
+    <t>bi-test</t>
+  </si>
+  <si>
+    <t>naresh</t>
+  </si>
+  <si>
+    <t>bee</t>
+  </si>
+  <si>
+    <t>kpglue</t>
+  </si>
+  <si>
+    <t>newtest</t>
+  </si>
+  <si>
+    <t>partially</t>
+  </si>
+  <si>
+    <t>glueall</t>
+  </si>
+  <si>
+    <t>glu</t>
+  </si>
+  <si>
+    <t>chargebeetest</t>
+  </si>
+  <si>
+    <t>prodtetst2</t>
+  </si>
+  <si>
+    <t>producttest</t>
+  </si>
+  <si>
+    <t>srigluetest</t>
+  </si>
+  <si>
+    <t>jyoti@e6x.io</t>
+  </si>
+  <si>
+    <t>akash@e6x.io</t>
+  </si>
+  <si>
+    <t>govindaraju@e6x.io</t>
+  </si>
+  <si>
+    <t>kumar@e6x.io</t>
+  </si>
+  <si>
+    <t>rajath@e6x.io</t>
+  </si>
+  <si>
+    <t>garvit@e6x.io</t>
+  </si>
+  <si>
+    <t>shubham.kumar@e6x.io</t>
+  </si>
+  <si>
+    <t>dasari.laxminaresh@e6x.io</t>
+  </si>
+  <si>
+    <t>vishal@e6x.io</t>
+  </si>
+  <si>
+    <t>karan@e6x.io</t>
+  </si>
+  <si>
+    <t>srinath@e6x.io</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>plt-infra</t>
+  </si>
+  <si>
+    <t>Query editor</t>
+  </si>
+  <si>
+    <t>Notebook</t>
+  </si>
+  <si>
+    <t>Catalogs</t>
+  </si>
+  <si>
+    <t>Clusters</t>
+  </si>
+  <si>
+    <t>Query history</t>
+  </si>
+  <si>
+    <t>Connectivity</t>
+  </si>
+  <si>
+    <t>Endpoints</t>
+  </si>
+  <si>
+    <t>IP sets</t>
+  </si>
+  <si>
+    <t>Workspaces</t>
+  </si>
+  <si>
+    <t>feb-27th</t>
+  </si>
+  <si>
+    <t>highqps</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>testt</t>
+  </si>
+  <si>
+    <t>feb-24th</t>
+  </si>
+  <si>
+    <t>feb-7th</t>
+  </si>
+  <si>
+    <t>pov</t>
+  </si>
+  <si>
+    <t>task@e6x.io</t>
+  </si>
+  <si>
+    <t>shubham@e6x.io</t>
+  </si>
+  <si>
+    <t>Suspended</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -435,18 +628,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="20.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -457,7 +700,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -465,10 +708,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.0"/>
+    <col min="2" max="2" customWidth="true" width="24.5703125"/>
+    <col min="3" max="3" customWidth="true" width="19.42578125"/>
+    <col min="4" max="4" customWidth="true" width="22.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -483,6 +726,328 @@
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -492,7 +1057,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
@@ -500,10 +1065,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.0"/>
+    <col min="2" max="2" customWidth="true" width="24.5703125"/>
+    <col min="3" max="3" customWidth="true" width="19.42578125"/>
+    <col min="4" max="4" customWidth="true" width="22.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -518,6 +1083,130 @@
       </c>
       <c r="D1" s="2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>80</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -535,9 +1224,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.42578125"/>
+    <col min="2" max="2" customWidth="true" width="28.0"/>
+    <col min="3" max="3" customWidth="true" width="30.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -552,13 +1241,13 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>10</v>
       </c>
     </row>

</xml_diff>